<commit_message>
reorganizing to allow for SQLite and SQL Server 2017 options
</commit_message>
<xml_diff>
--- a/rieslings.xlsx
+++ b/rieslings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -28,76 +28,61 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Trimbach Réserve Riesling 2009</t>
-  </si>
-  <si>
-    <t>Kuentz Riesling 2015</t>
-  </si>
-  <si>
-    <t>Hugel Riesling Classic 2014</t>
-  </si>
-  <si>
-    <t>Domaine Ostertag Riesling Clos Mathis 2015</t>
-  </si>
-  <si>
-    <t>Domaine Ostertag Fronholz Riesling 2015</t>
-  </si>
-  <si>
-    <t>Domaines Schlumberger Kessler Riesling Grand Cru 2012</t>
-  </si>
-  <si>
-    <t>Koenig Riesling Kp M 2015</t>
-  </si>
-  <si>
-    <t>Trimbach Riesling 2013</t>
+    <t>Joseph Cattin Riesling 2014</t>
+  </si>
+  <si>
+    <t>Schieferkopf Lieu-Dit Fels Riesling 2011</t>
+  </si>
+  <si>
+    <t>Gustave Lorentz Réserve Riesling 2014</t>
+  </si>
+  <si>
+    <t>Boeckel Wiebelsberg Riesling 2012</t>
+  </si>
+  <si>
+    <t>Baron de Hoen Réserve Riesling 2014</t>
+  </si>
+  <si>
+    <t>Cave de Beblenheim Heimberger Réserve Riesling</t>
+  </si>
+  <si>
+    <t>Gustave Lorentz Riesling Cuvee Amethyste</t>
+  </si>
+  <si>
+    <t>Henri Ehrhart Réserve Particulière Riesling 2013</t>
+  </si>
+  <si>
+    <t>Trimbach Riesling 2012</t>
+  </si>
+  <si>
+    <t>Boeckel Brandluft Riesling 2012</t>
+  </si>
+  <si>
+    <t>Jean Geiler Réserve Particulière Riesling 2013</t>
   </si>
   <si>
     <t>Willm Réserve Riesling</t>
   </si>
   <si>
-    <t>Léon Beyer Réserve Riesling 2015</t>
-  </si>
-  <si>
-    <t>Boeckel Brandluft Vieilles Vignes Riesling 2013</t>
-  </si>
-  <si>
-    <t>Schieferkopf Lieu-Dit Fels Riesling 2011</t>
-  </si>
-  <si>
-    <t>Domaine Marc Kreydenweiss G. C. Kastelberg Riesling 2013</t>
-  </si>
-  <si>
-    <t>Baron de Hoen Réserve Riesling 2014</t>
-  </si>
-  <si>
-    <t>Pfaff Riesling Cuvee Jupiter Alsace Aoc</t>
-  </si>
-  <si>
-    <t>Joseph Cattin Riesling 2015</t>
-  </si>
-  <si>
-    <t>Kuentz-Bas Trois Chateaux Pfersigberg Riesling 2012</t>
-  </si>
-  <si>
-    <t>Emile Beyer Pfersigberg Riesling 2012</t>
-  </si>
-  <si>
-    <t>Cave Vinicole Du Vieil Armand Riesling 2015</t>
-  </si>
-  <si>
     <t>J. Fritsch Riesling 2014</t>
   </si>
   <si>
-    <t>J.M. Sohler Heissenberg Riesling 2015</t>
-  </si>
-  <si>
-    <t>Domaine Allimant-Laugner Riesling 2014</t>
-  </si>
-  <si>
-    <t>Jean Biecher &amp; Fils Schoenenbourg Riesling 2014</t>
+    <t>Hugel &amp; Fils Jubilee Riesling 2009</t>
+  </si>
+  <si>
+    <t>Pierre Sparr Lieu Dit Altenbourg Riesling 2013</t>
+  </si>
+  <si>
+    <t>Koenig Riesling Kp M 2014</t>
+  </si>
+  <si>
+    <t>Pierre Sparr Schoenenbourg Riesling 2011</t>
   </si>
   <si>
     <t>Domaine Pfister Silberberg Sélection de Grains Nobles Riesling 2007</t>
+  </si>
+  <si>
+    <t>Clos St. Landelin Vorbourg Sélection de Grains Nobles Riesling 2007</t>
   </si>
 </sst>
 </file>
@@ -446,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -475,12 +460,14 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2">
+        <v>5</v>
+      </c>
       <c r="C2" s="2">
         <v>750</v>
       </c>
       <c r="D2" s="3">
-        <v>25.95</v>
+        <v>14.95</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -488,13 +475,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2">
         <v>750</v>
       </c>
       <c r="D3" s="3">
-        <v>23.4</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -502,13 +489,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
         <v>750</v>
       </c>
       <c r="D4" s="3">
-        <v>28.55</v>
+        <v>18.95</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -516,13 +503,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
         <v>750</v>
       </c>
       <c r="D5" s="3">
-        <v>48.05</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -530,13 +517,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2">
         <v>750</v>
       </c>
       <c r="D6" s="3">
-        <v>49.15</v>
+        <v>14.95</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -544,13 +531,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2">
         <v>750</v>
       </c>
       <c r="D7" s="3">
-        <v>27.95</v>
+        <v>15.95</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -558,13 +545,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2">
         <v>750</v>
       </c>
       <c r="D8" s="3">
-        <v>19.95</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -572,13 +559,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2">
         <v>750</v>
       </c>
       <c r="D9" s="3">
-        <v>23.95</v>
+        <v>16.95</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -586,13 +573,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2">
         <v>750</v>
       </c>
       <c r="D10" s="3">
-        <v>15.95</v>
+        <v>21.95</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -600,13 +587,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C11" s="2">
         <v>750</v>
       </c>
       <c r="D11" s="3">
-        <v>19.95</v>
+        <v>14.75</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -614,13 +601,13 @@
         <v>14</v>
       </c>
       <c r="B12" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2">
         <v>750</v>
       </c>
       <c r="D12" s="3">
-        <v>29</v>
+        <v>14.95</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -628,13 +615,13 @@
         <v>15</v>
       </c>
       <c r="B13" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2">
         <v>750</v>
       </c>
       <c r="D13" s="3">
-        <v>49</v>
+        <v>15.95</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -642,13 +629,13 @@
         <v>16</v>
       </c>
       <c r="B14" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2">
         <v>750</v>
       </c>
       <c r="D14" s="3">
-        <v>79</v>
+        <v>17.25</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -656,13 +643,13 @@
         <v>17</v>
       </c>
       <c r="B15" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" s="2">
         <v>750</v>
       </c>
       <c r="D15" s="3">
-        <v>12.75</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -670,13 +657,13 @@
         <v>18</v>
       </c>
       <c r="B16" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C16" s="2">
         <v>750</v>
       </c>
       <c r="D16" s="3">
-        <v>15.5</v>
+        <v>16.95</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -684,13 +671,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C17" s="2">
         <v>750</v>
       </c>
       <c r="D17" s="3">
-        <v>15.95</v>
+        <v>18.95</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -698,13 +685,13 @@
         <v>20</v>
       </c>
       <c r="B18" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C18" s="2">
         <v>750</v>
       </c>
       <c r="D18" s="3">
-        <v>55</v>
+        <v>22.95</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -712,13 +699,13 @@
         <v>21</v>
       </c>
       <c r="B19" s="2">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C19" s="2">
-        <v>750</v>
+        <v>500</v>
       </c>
       <c r="D19" s="3">
-        <v>59</v>
+        <v>56.25</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -726,83 +713,13 @@
         <v>22</v>
       </c>
       <c r="B20" s="2">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="C20" s="2">
-        <v>750</v>
+        <v>500</v>
       </c>
       <c r="D20" s="3">
-        <v>16.75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="2">
-        <v>8</v>
-      </c>
-      <c r="C21" s="2">
-        <v>750</v>
-      </c>
-      <c r="D21" s="3">
-        <v>17.25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="2">
-        <v>8</v>
-      </c>
-      <c r="C22" s="2">
-        <v>750</v>
-      </c>
-      <c r="D22" s="3">
-        <v>18.95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="2">
-        <v>10</v>
-      </c>
-      <c r="C23" s="2">
-        <v>750</v>
-      </c>
-      <c r="D23" s="3">
-        <v>18.95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="2">
-        <v>10</v>
-      </c>
-      <c r="C24" s="2">
-        <v>750</v>
-      </c>
-      <c r="D24" s="3">
-        <v>23.95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="2">
-        <v>100</v>
-      </c>
-      <c r="C25" s="2">
-        <v>500</v>
-      </c>
-      <c r="D25" s="3">
-        <v>56.25</v>
+        <v>51.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>